<commit_message>
Add two atributes 'Materia'
</commit_message>
<xml_diff>
--- a/db/Profesor.xlsx
+++ b/db/Profesor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PosGrado\Proyecto Titulacion\Timetabling\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A51478-F028-4A7D-AB74-635AC822D580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAC80DA-00FA-4080-A185-539745E43428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9285" yWindow="5535" windowWidth="28785" windowHeight="15345" xr2:uid="{5C1DD6D8-1001-4079-A3F5-95F5066F8827}"/>
+    <workbookView xWindow="3975" yWindow="4695" windowWidth="28785" windowHeight="15345" xr2:uid="{5C1DD6D8-1001-4079-A3F5-95F5066F8827}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="61">
   <si>
     <t>profesor_id</t>
   </si>
@@ -45,9 +45,6 @@
     <t>apellido</t>
   </si>
   <si>
-    <t>especialidad</t>
-  </si>
-  <si>
     <t>categoria</t>
   </si>
   <si>
@@ -204,28 +201,22 @@
     <t>Piano</t>
   </si>
   <si>
-    <t>Cello</t>
-  </si>
-  <si>
     <t>Loayza</t>
   </si>
   <si>
-    <t>Violín</t>
-  </si>
-  <si>
-    <t>Clarinete</t>
-  </si>
-  <si>
-    <t>Oboe</t>
-  </si>
-  <si>
     <t>Canto</t>
   </si>
   <si>
-    <t>Viola</t>
-  </si>
-  <si>
-    <t>VIolín</t>
+    <t>seccion</t>
+  </si>
+  <si>
+    <t>Cuerda</t>
+  </si>
+  <si>
+    <t>Viento</t>
+  </si>
+  <si>
+    <t>Percusion</t>
   </si>
 </sst>
 </file>
@@ -580,7 +571,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I3"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,10 +590,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -610,16 +601,16 @@
         <v>1001</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -627,16 +618,16 @@
         <v>1002</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -644,16 +635,16 @@
         <v>1003</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -661,16 +652,16 @@
         <v>1004</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -678,16 +669,16 @@
         <v>1005</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -695,16 +686,16 @@
         <v>1006</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -712,16 +703,16 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -729,16 +720,16 @@
         <v>1008</v>
       </c>
       <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -746,16 +737,16 @@
         <v>1009</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -763,16 +754,16 @@
         <v>1010</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -780,16 +771,16 @@
         <v>1011</v>
       </c>
       <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -797,16 +788,16 @@
         <v>1012</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
         <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -814,16 +805,16 @@
         <v>1013</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
         <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -831,16 +822,16 @@
         <v>1014</v>
       </c>
       <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -848,16 +839,16 @@
         <v>1015</v>
       </c>
       <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -865,16 +856,16 @@
         <v>1016</v>
       </c>
       <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
         <v>42</v>
       </c>
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -882,16 +873,16 @@
         <v>1017</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -899,16 +890,16 @@
         <v>1018</v>
       </c>
       <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -916,16 +907,16 @@
         <v>1019</v>
       </c>
       <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
         <v>31</v>
       </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -933,16 +924,16 @@
         <v>1020</v>
       </c>
       <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
         <v>33</v>
       </c>
-      <c r="C21" t="s">
-        <v>34</v>
-      </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -950,16 +941,16 @@
         <v>1021</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -967,16 +958,16 @@
         <v>1022</v>
       </c>
       <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
         <v>38</v>
       </c>
-      <c r="C23" t="s">
-        <v>39</v>
-      </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -984,16 +975,16 @@
         <v>1023</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1001,16 +992,16 @@
         <v>1024</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1018,16 +1009,16 @@
         <v>1025</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1035,21 +1026,21 @@
         <v>1026</v>
       </c>
       <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
         <v>48</v>
       </c>
-      <c r="C27" t="s">
-        <v>49</v>
-      </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>